<commit_message>
Update Investigation for correctness
</commit_message>
<xml_diff>
--- a/tests/fixtures/testARC_licenseMissing/isa.investigation.xlsx
+++ b/tests/fixtures/testARC_licenseMissing/isa.investigation.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EE6FC6-1EE5-4577-BF89-E763B4973787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="isa_investigation" state="visible" r:id="rId4"/>
+    <sheet name="isa_investigation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -34,9 +51,6 @@
     <t>Investigation Identifier</t>
   </si>
   <si>
-    <t>testARC_licenseMissing</t>
-  </si>
-  <si>
     <t>Investigation Title</t>
   </si>
   <si>
@@ -107,19 +121,60 @@
   </si>
   <si>
     <t>Investigation Person Roles Term Source REF</t>
+  </si>
+  <si>
+    <t>Person X</t>
+  </si>
+  <si>
+    <t>per@son.X</t>
+  </si>
+  <si>
+    <t>http://orcid.org/0000-0001-5109-3700</t>
+  </si>
+  <si>
+    <t>0000-0001-5109-3700</t>
+  </si>
+  <si>
+    <t>Person Y</t>
+  </si>
+  <si>
+    <t>per@son.Y</t>
+  </si>
+  <si>
+    <t>testARC_correctOrcid</t>
+  </si>
+  <si>
+    <t>Comment[ORCID]</t>
+  </si>
+  <si>
+    <t>Person Z</t>
+  </si>
+  <si>
+    <t>per@son.Z</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-5109-3700</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,14 +194,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,36 +516,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -495,132 +565,195 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{631E10BF-1F5C-46E6-A644-E3FF6F2C9128}"/>
+    <hyperlink ref="B32" r:id="rId2" xr:uid="{4C4E852B-4AA9-4695-A6EA-6FE5F9B10728}"/>
+    <hyperlink ref="C24" r:id="rId3" xr:uid="{91790182-1BB2-4150-983B-00593AE00F15}"/>
+    <hyperlink ref="D24" r:id="rId4" xr:uid="{B8ABF616-CBC3-4FC4-9C80-E2FD90A60557}"/>
+    <hyperlink ref="C32" r:id="rId5" xr:uid="{44D8F952-C1B4-4E37-BB11-4B47BC0E9710}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>